<commit_message>
Trailing white space causes bug.
</commit_message>
<xml_diff>
--- a/test/input-files/42.xlsx
+++ b/test/input-files/42.xlsx
@@ -336,7 +336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -350,6 +350,12 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"test"&amp;" with trailing white space "</f>
+        <v xml:space="preserve">test with trailing white space </v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Empty cells now return null
</commit_message>
<xml_diff>
--- a/test/input-files/42.xlsx
+++ b/test/input-files/42.xlsx
@@ -336,10 +336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -356,6 +356,12 @@
         <v xml:space="preserve">test with trailing white space </v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>